<commit_message>
added the fireontop grid so all the maps are compatible with the new alg
</commit_message>
<xml_diff>
--- a/map/MapDesigns.xlsx
+++ b/map/MapDesigns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\Reinforcement-Learning-Malmo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\FireEscape\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C087B134-34D5-4063-B7E8-5E30C67B8FFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94283A21-672F-4611-BFEE-EA2F4758E4D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FDBFA2F1-4C98-476F-A615-69E8EC84A2D0}"/>
+    <workbookView xWindow="20280" yWindow="3270" windowWidth="16395" windowHeight="15780" xr2:uid="{FDBFA2F1-4C98-476F-A615-69E8EC84A2D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="9">
   <si>
     <t>Map 1</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Map 4</t>
+  </si>
+  <si>
+    <t>Map 7</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -177,6 +183,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B1C20E-8CE6-49CC-88EA-E7B79E8805AC}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,6 +706,9 @@
       <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C12" s="4"/>
@@ -703,6 +716,13 @@
       <c r="E12" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C13" s="5"/>
@@ -710,6 +730,13 @@
       <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C14" s="3" t="s">
@@ -721,6 +748,27 @@
       <c r="E14" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="H14" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C15" s="3" t="s">
@@ -728,6 +776,15 @@
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C16" s="3" t="s">
@@ -739,16 +796,51 @@
       <c r="E16" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="H18" s="12"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated spreadsheet with map9 info
</commit_message>
<xml_diff>
--- a/map/MapDesigns.xlsx
+++ b/map/MapDesigns.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27815"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\FireEscape\map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/groot/school/cs175/FireEscape/map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94283A21-672F-4611-BFEE-EA2F4758E4D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="3270" windowWidth="16395" windowHeight="15780" xr2:uid="{FDBFA2F1-4C98-476F-A615-69E8EC84A2D0}"/>
+    <workbookView xWindow="10540" yWindow="1200" windowWidth="18260" windowHeight="15780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
   <si>
     <t>Map 1</t>
   </si>
@@ -58,13 +63,22 @@
   </si>
   <si>
     <t>-&gt;</t>
+  </si>
+  <si>
+    <t>Map 9 (P = Elevated Platform)</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>*P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +109,12 @@
     </font>
     <font>
       <sz val="43"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -154,24 +174,42 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -187,6 +225,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,20 +542,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B1C20E-8CE6-49CC-88EA-E7B79E8805AC}">
-  <dimension ref="A1:P25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="57" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="34" width="15.140625" customWidth="1"/>
+    <col min="1" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="34" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -556,7 +598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -581,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="4" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -602,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="5" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -623,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="6" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -650,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="7" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
@@ -662,7 +704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="8" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -677,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="9" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
@@ -689,14 +731,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="10" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="11" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
@@ -709,8 +751,11 @@
       <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
@@ -723,8 +768,19 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
-    </row>
-    <row r="13" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P12" s="12"/>
+      <c r="Q12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="12"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="15"/>
+    </row>
+    <row r="13" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
@@ -737,8 +793,19 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
       <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="U13" s="17"/>
+      <c r="V13" s="15"/>
+    </row>
+    <row r="14" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
@@ -769,8 +836,19 @@
       <c r="N14" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" s="5"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="15"/>
+    </row>
+    <row r="15" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
@@ -785,8 +863,19 @@
       <c r="N15" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S15" s="12"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="15"/>
+    </row>
+    <row r="16" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="C16" s="3" t="s">
         <v>2</v>
       </c>
@@ -805,8 +894,17 @@
       <c r="N16" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P16" s="12"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="15"/>
+    </row>
+    <row r="17" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -816,8 +914,21 @@
       <c r="N17" s="14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P17" s="12"/>
+      <c r="Q17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T17" s="5"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="16"/>
+    </row>
+    <row r="18" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="H18" s="12"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
@@ -825,8 +936,21 @@
       <c r="L18" s="12"/>
       <c r="M18" s="11"/>
       <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U18" s="17"/>
+      <c r="V18" s="15"/>
+    </row>
+    <row r="19" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
@@ -834,15 +958,19 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="8:14" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+    </row>
+    <row r="20" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes for map9 so the spreadsheet and the map in game is the same
</commit_message>
<xml_diff>
--- a/map/MapDesigns.xlsx
+++ b/map/MapDesigns.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27815"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/groot/school/cs175/FireEscape/map/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\FireEscape\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C37008-377A-4C3B-8353-FA2114017D05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="1200" windowWidth="18260" windowHeight="15780"/>
+    <workbookView xWindow="17685" yWindow="4800" windowWidth="15900" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,24 +20,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
   <si>
     <t>Map 1</t>
   </si>
@@ -72,12 +67,102 @@
   </si>
   <si>
     <t>*P</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>286</t>
+  </si>
+  <si>
+    <t>263</t>
+  </si>
+  <si>
+    <t>284</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>326</t>
+  </si>
+  <si>
+    <t>262</t>
+  </si>
+  <si>
+    <t>283</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>346</t>
+  </si>
+  <si>
+    <t>348</t>
+  </si>
+  <si>
+    <t>349</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>285</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>327</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>&lt;-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -226,9 +311,12 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,20 +630,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="57" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView tabSelected="1" topLeftCell="H11" zoomScale="57" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="14.5" customWidth="1"/>
-    <col min="12" max="34" width="15.1640625" customWidth="1"/>
+    <col min="1" max="11" width="14.42578125" customWidth="1"/>
+    <col min="12" max="24" width="15.140625" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" customWidth="1"/>
+    <col min="26" max="34" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -598,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -623,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -643,8 +733,17 @@
       <c r="P4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V4" s="12"/>
+      <c r="W4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="19"/>
+    </row>
+    <row r="5" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -664,8 +763,17 @@
       <c r="P5" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V5" s="20"/>
+      <c r="W5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+    </row>
+    <row r="6" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -691,8 +799,15 @@
       <c r="P6" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V6" s="20"/>
+      <c r="W6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="12"/>
+    </row>
+    <row r="7" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
@@ -703,8 +818,17 @@
       <c r="P7" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V7" s="11"/>
+      <c r="W7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+    </row>
+    <row r="8" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -718,8 +842,19 @@
       <c r="P8" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V8" s="12"/>
+      <c r="W8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="X8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" s="20"/>
+    </row>
+    <row r="9" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
@@ -730,15 +865,35 @@
       <c r="K9" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V9" s="12"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="20"/>
+    </row>
+    <row r="10" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="V10" s="11"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
@@ -755,7 +910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
@@ -776,11 +931,21 @@
         <v>2</v>
       </c>
       <c r="S12" s="12"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="15"/>
-    </row>
-    <row r="13" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="T12" s="19"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="X12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
@@ -802,10 +967,22 @@
       <c r="T13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="U13" s="17"/>
-      <c r="V13" s="15"/>
-    </row>
-    <row r="14" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="U13" s="16"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="X13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
@@ -836,19 +1013,25 @@
       <c r="N14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="P14" s="5"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="11" t="s">
         <v>11</v>
       </c>
       <c r="S14" s="5"/>
       <c r="T14" s="12"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="15"/>
-    </row>
-    <row r="15" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="U14" s="16"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y14" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z14" s="12"/>
+    </row>
+    <row r="15" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
@@ -870,12 +1053,26 @@
       <c r="R15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="S15" s="12"/>
+      <c r="S15" s="11"/>
       <c r="T15" s="11"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="15"/>
-    </row>
-    <row r="16" spans="1:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="U15" s="16"/>
+      <c r="V15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="X15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z15" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C16" s="3" t="s">
         <v>2</v>
       </c>
@@ -895,16 +1092,24 @@
         <v>2</v>
       </c>
       <c r="P16" s="12"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="S16" s="5"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="3"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="15"/>
-    </row>
-    <row r="17" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="U16" s="16"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z16" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -925,10 +1130,22 @@
         <v>10</v>
       </c>
       <c r="T17" s="5"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="16"/>
-    </row>
-    <row r="18" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="U17" s="16"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="X17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z17" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="H18" s="12"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
@@ -947,10 +1164,20 @@
       <c r="T18" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="U18" s="17"/>
-      <c r="V18" s="15"/>
-    </row>
-    <row r="19" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="U18" s="16"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y18" s="11">
+        <v>221</v>
+      </c>
+      <c r="Z18" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
@@ -958,16 +1185,20 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="12"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
       <c r="T19" s="18"/>
       <c r="U19" s="15"/>
       <c r="V19" s="15"/>
     </row>
-    <row r="20" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="8:22" ht="72" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upload map12 (doesn't converge)
</commit_message>
<xml_diff>
--- a/map/MapDesigns.xlsx
+++ b/map/MapDesigns.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DesmenH_RedSpecter\Source\Repos\FireEscape\map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Malmo\FireEscape\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C37008-377A-4C3B-8353-FA2114017D05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43886D1D-B8FE-44BE-81A1-59274BA18C4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17685" yWindow="4800" windowWidth="15900" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="7314" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="43">
   <si>
     <t>Map 1</t>
   </si>
@@ -157,13 +157,16 @@
   </si>
   <si>
     <t>&lt;-</t>
+  </si>
+  <si>
+    <t>map 12 (fail)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +207,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,8 +278,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -290,11 +332,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -317,6 +387,16 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,21 +711,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AL25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H11" zoomScale="57" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="W10" zoomScale="57" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="24" width="15.140625" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
-    <col min="26" max="34" width="15.140625" customWidth="1"/>
+    <col min="1" max="11" width="14.41796875" customWidth="1"/>
+    <col min="12" max="24" width="15.15625" customWidth="1"/>
+    <col min="25" max="25" width="15.83984375" customWidth="1"/>
+    <col min="26" max="34" width="15.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.05">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,7 +736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="2" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -688,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -713,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="4" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -743,7 +823,7 @@
       <c r="Y4" s="12"/>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="5" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -773,7 +853,7 @@
       <c r="Y5" s="11"/>
       <c r="Z5" s="11"/>
     </row>
-    <row r="6" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="6" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -807,7 +887,7 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="12"/>
     </row>
-    <row r="7" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="7" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
@@ -828,7 +908,7 @@
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
     </row>
-    <row r="8" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="8" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -854,7 +934,7 @@
       </c>
       <c r="Z8" s="20"/>
     </row>
-    <row r="9" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="9" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
@@ -875,7 +955,7 @@
       </c>
       <c r="Z9" s="20"/>
     </row>
-    <row r="10" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="10" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
@@ -893,7 +973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="11" spans="1:38" ht="72" customHeight="1" x14ac:dyDescent="1.95">
       <c r="C11" s="4" t="s">
         <v>2</v>
       </c>
@@ -909,8 +989,11 @@
       <c r="P11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AF11" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="3" t="s">
@@ -944,8 +1027,18 @@
       <c r="Z12" s="19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC12" s="22"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="22"/>
+      <c r="AF12" s="23"/>
+      <c r="AG12" s="22"/>
+      <c r="AH12" s="23"/>
+      <c r="AI12" s="23"/>
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="23"/>
+      <c r="AL12" s="22"/>
+    </row>
+    <row r="13" spans="1:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
@@ -981,8 +1074,18 @@
       <c r="Z13" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="24"/>
+      <c r="AE13" s="25"/>
+      <c r="AF13" s="25"/>
+      <c r="AG13" s="24"/>
+      <c r="AH13" s="24"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="24"/>
+      <c r="AK13" s="24"/>
+      <c r="AL13" s="24"/>
+    </row>
+    <row r="14" spans="1:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1030,8 +1133,18 @@
         <v>26</v>
       </c>
       <c r="Z14" s="12"/>
-    </row>
-    <row r="15" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC14" s="27"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="24"/>
+      <c r="AG14" s="24"/>
+      <c r="AH14" s="24"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="24"/>
+      <c r="AK14" s="24"/>
+      <c r="AL14" s="26"/>
+    </row>
+    <row r="15" spans="1:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1071,8 +1184,26 @@
       <c r="Z15" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC15" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI15" s="26"/>
+      <c r="AJ15" s="24"/>
+      <c r="AK15" s="24"/>
+      <c r="AL15" s="26"/>
+    </row>
+    <row r="16" spans="1:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="C16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1108,8 +1239,18 @@
       <c r="Z16" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC16" s="26"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="24"/>
+      <c r="AG16" s="24"/>
+      <c r="AH16" s="29"/>
+      <c r="AI16" s="29"/>
+      <c r="AJ16" s="26"/>
+      <c r="AK16" s="24"/>
+      <c r="AL16" s="24"/>
+    </row>
+    <row r="17" spans="8:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
@@ -1144,8 +1285,20 @@
       <c r="Z17" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC17" s="24"/>
+      <c r="AD17" s="26"/>
+      <c r="AE17" s="24"/>
+      <c r="AF17" s="24"/>
+      <c r="AG17" s="24"/>
+      <c r="AH17" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI17" s="26"/>
+      <c r="AJ17" s="24"/>
+      <c r="AK17" s="24"/>
+      <c r="AL17" s="26"/>
+    </row>
+    <row r="18" spans="8:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="H18" s="12"/>
       <c r="I18" s="11"/>
       <c r="J18" s="12"/>
@@ -1176,8 +1329,24 @@
       <c r="Z18" s="13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+      <c r="AG18" s="26"/>
+      <c r="AH18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI18" s="24"/>
+      <c r="AJ18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK18" s="24"/>
+      <c r="AL18" s="26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="8:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="2">
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
@@ -1192,13 +1361,36 @@
       <c r="T19" s="18"/>
       <c r="U19" s="15"/>
       <c r="V19" s="15"/>
-    </row>
-    <row r="20" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="8:26" ht="72" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="24"/>
+      <c r="AG19" s="26"/>
+      <c r="AH19" s="26"/>
+      <c r="AI19" s="24"/>
+      <c r="AJ19" s="24"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="26"/>
+    </row>
+    <row r="20" spans="8:38" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="1.35">
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24"/>
+      <c r="AE20" s="26"/>
+      <c r="AF20" s="24"/>
+      <c r="AG20" s="24"/>
+      <c r="AH20" s="24"/>
+      <c r="AI20" s="24"/>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="25"/>
+      <c r="AL20" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="8:38" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="22" spans="8:38" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="23" spans="8:38" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="8:38" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="8:38" ht="72" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>